<commit_message>
shorten definitions that caused errors in download
</commit_message>
<xml_diff>
--- a/spreadsheet_vocabs/WaMDaM_CVs_Dec2018.xlsx
+++ b/spreadsheet_vocabs/WaMDaM_CVs_Dec2018.xlsx
@@ -4752,34 +4752,34 @@
     <t>SWMM</t>
   </si>
   <si>
-    <t>WEAP ("Water Evaluation And Planning" system) is a user-friendly software tool that takes an integrated approach to water resources planning.</t>
-  </si>
-  <si>
     <t>http://www.weap21.org/</t>
   </si>
   <si>
     <t>http://riverware.org/</t>
   </si>
   <si>
-    <t>RiverWare is a river system modeling tool. It is an ideal platform for operational decision-making, responsive forecasting, operational policy evaluation, system optimization, water accounting, water rights administration, and long-term resource planning. The wide range of applications is made possible by a choice of computational timesteps ranging from 1 hour to 1 year.</t>
-  </si>
-  <si>
     <t>https://www.epa.gov/water-research/epanet</t>
   </si>
   <si>
-    <t>EPANET is used throughout the world to model water distribution systems. This software application is used to perform extended-period simulation of the hydraulic and water quality behavior within pressurized pipe networks, which consist of pipes, nodes (junctions), pumps, valves,  storage tanks, and reservoirs. It can be used to track the flow of water in each pipe, the pressure at each node, the height of the water in each tank, a chemical concentration, the age of the water, and source tracing throughout the network during a simulation period.</t>
-  </si>
-  <si>
     <t>https://www.epa.gov/water-research/storm-water-management-model-swmm</t>
   </si>
   <si>
-    <t>EPA's Stormwater Management Model (SWMM) is used for single event or long-term simulations of water runoff quantity and quality in primarily urban areas–although there are also many applications that can be used for drainage systems in non-urban areas. It is used throughout the world for planning, analysis, and design related to stormwater runoff, combined and sanitary sewers, and other drainage systems. SWMM was developed to help support local, state, and national stormwater management objectives to reduce runoff through infiltration and retention, and help to reduce discharges that cause impairment of our Nation’s waterbodies.</t>
-  </si>
-  <si>
     <t>https://github.com/ayman510/WASH</t>
   </si>
   <si>
     <t>Systems Modeling to Improve River, Riparian and Wetlands Habitat Quality and Area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Water Evaluation And Planning system </t>
+  </si>
+  <si>
+    <t>RiverWare is a river system modeling tool</t>
+  </si>
+  <si>
+    <t>EPANET is used throughout the world to model water distribution systems.</t>
+  </si>
+  <si>
+    <t>EPAs Stormwater Management Model SWMM</t>
   </si>
 </sst>
 </file>
@@ -5244,7 +5244,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
@@ -5459,6 +5459,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -5467,13 +5470,6 @@
     <cellStyle name="Normal 3" xfId="3"/>
   </cellStyles>
   <dxfs count="19">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -5550,6 +5546,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5953,15 +5956,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="102.28515625" style="52" customWidth="1"/>
+    <col min="4" max="7" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -5971,7 +5977,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="66" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -5994,7 +6000,7 @@
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="67" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -6017,13 +6023,13 @@
       <c r="B3" s="8" t="s">
         <v>1549</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>1554</v>
+      <c r="C3" s="52" t="s">
+        <v>1560</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="G3" s="9"/>
     </row>
@@ -6034,13 +6040,13 @@
       <c r="B4" s="8" t="s">
         <v>1550</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>1557</v>
+      <c r="C4" s="52" t="s">
+        <v>1561</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="G4" s="9"/>
     </row>
@@ -6051,13 +6057,13 @@
       <c r="B5" s="8" t="s">
         <v>1551</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>1563</v>
+      <c r="C5" s="52" t="s">
+        <v>1559</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9" t="s">
-        <v>1562</v>
+        <v>1558</v>
       </c>
       <c r="G5" s="9"/>
     </row>
@@ -6068,11 +6074,11 @@
       <c r="B6" t="s">
         <v>1552</v>
       </c>
-      <c r="C6" t="s">
-        <v>1559</v>
+      <c r="C6" s="52" t="s">
+        <v>1562</v>
       </c>
       <c r="F6" t="s">
-        <v>1558</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -6082,16 +6088,19 @@
       <c r="B7" t="s">
         <v>1553</v>
       </c>
-      <c r="C7" t="s">
-        <v>1561</v>
+      <c r="C7" s="52" t="s">
+        <v>1563</v>
       </c>
       <c r="F7" t="s">
-        <v>1560</v>
-      </c>
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="84"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A20">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -12088,7 +12097,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -13330,7 +13339,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A15">
-    <cfRule type="duplicateValues" dxfId="4" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="9"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -13530,7 +13539,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A17">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -13766,7 +13775,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A22">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -13907,7 +13916,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A15">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -14017,7 +14026,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A20">
-    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -14400,7 +14409,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A1048576">
-    <cfRule type="duplicateValues" dxfId="17" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -14543,7 +14552,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A25">
-    <cfRule type="duplicateValues" dxfId="16" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -15358,7 +15367,7 @@
     <row r="71" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="A3:A65">
-    <cfRule type="duplicateValues" dxfId="15" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="7"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -17114,7 +17123,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A100">
-    <cfRule type="duplicateValues" dxfId="14" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -18798,10 +18807,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B79">
-    <cfRule type="duplicateValues" dxfId="13" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A200">
-    <cfRule type="duplicateValues" dxfId="12" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -26500,22 +26509,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A1048576">
-    <cfRule type="duplicateValues" dxfId="11" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B198 B200:B202 B204:B1048576">
-    <cfRule type="duplicateValues" dxfId="10" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D160:D1048576 D1:D158">
-    <cfRule type="duplicateValues" dxfId="9" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D159">
-    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B199">
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B203">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>